<commit_message>
HardCode Patient check from Excel working
</commit_message>
<xml_diff>
--- a/CVGreenWare/Excel Docs/Patient.xlsx
+++ b/CVGreenWare/Excel Docs/Patient.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,10 +86,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -404,18 +405,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="3" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -428,7 +429,7 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="3">
         <v>56</v>
       </c>
       <c r="D1" t="s">
@@ -448,7 +449,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>44</v>
       </c>
       <c r="D2" t="s">
@@ -463,9 +464,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{BF270770-5E5E-4239-B3A5-B785F0F4CAA4}"/>
+    <hyperlink ref="F1" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>